<commit_message>
mejora de formulario de pedidos
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\xampp\osiris\osiris\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237DFE8E-051B-4322-BEBE-ADBAE93B8BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A548E952-23C7-4BE7-9ABB-6173FC410D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{3E32DC6F-2995-40D6-8CCF-7810F53B053D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>pedidos</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>precio_total_sugerido</t>
+  </si>
+  <si>
+    <t>precio_producto2</t>
+  </si>
+  <si>
+    <t>precio_compra</t>
   </si>
 </sst>
 </file>
@@ -3395,13 +3401,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>369794</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>123266</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1262213</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>164726</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3477,13 +3483,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>816004</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>156882</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>840441</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>123266</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3530,13 +3536,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1266265</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>33618</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3581,13 +3587,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>874059</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1101193</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>100423</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3652,13 +3658,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>40341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>760534</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>73529</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3723,13 +3729,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1627094</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>103094</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>16463</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>136282</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3794,13 +3800,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>121024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1827334</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>154211</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4307,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6DFE57-A63A-488A-BCC0-E7D282D3CD7B}">
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4459,8 +4465,8 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
-        <v>44</v>
+      <c r="B21" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>45</v>
@@ -4471,7 +4477,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>23</v>
@@ -4481,7 +4487,15 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="F23" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
proveedores e inicio de producto
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="9180" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="119">
   <si>
     <t>pedidos</t>
   </si>
@@ -103,9 +103,6 @@
     <t>direccion_proveedor</t>
   </si>
   <si>
-    <t>telefono_proveedor</t>
-  </si>
-  <si>
     <t>estado</t>
   </si>
   <si>
@@ -374,6 +371,27 @@
   </si>
   <si>
     <t>cuenta_cobro</t>
+  </si>
+  <si>
+    <t>categorias</t>
+  </si>
+  <si>
+    <t>id_cat</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>id_cat1</t>
+  </si>
+  <si>
+    <t>contacto_proveedor</t>
+  </si>
+  <si>
+    <t>nom_vendedor</t>
+  </si>
+  <si>
+    <t>telefono_vendedor</t>
   </si>
 </sst>
 </file>
@@ -424,7 +442,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +509,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -504,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -552,6 +576,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,13 +999,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>125982</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1425820</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>178649</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1182,13 +1207,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>62668</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1234,13 +1259,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1389529</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1893794</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>51462</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1555,13 +1580,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>294369</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>156451</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1626,13 +1651,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1620371</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1847505</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>6291</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1697,13 +1722,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>69477</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>35857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>296611</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>69044</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1768,13 +1793,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1623474</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>120681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1850608</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>142662</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3257,13 +3282,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1860176</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>193516</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>33188</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3540,15 +3565,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>369794</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>123266</xdr:rowOff>
+      <xdr:colOff>325832</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167228</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1262213</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>164726</xdr:rowOff>
+      <xdr:colOff>1218251</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>25515</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3563,8 +3588,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="627529" y="5221942"/>
-          <a:ext cx="892419" cy="579343"/>
+          <a:off x="582274" y="5918863"/>
+          <a:ext cx="892419" cy="590979"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
           <a:avLst/>
@@ -3622,15 +3647,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>816004</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
+      <xdr:colOff>772042</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>10344</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>840441</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>123266</xdr:rowOff>
+      <xdr:colOff>796479</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167228</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3647,8 +3672,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1073739" y="3978088"/>
-          <a:ext cx="24437" cy="1243854"/>
+          <a:off x="1028484" y="4648286"/>
+          <a:ext cx="24437" cy="1270577"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3675,15 +3700,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1266265</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
+      <xdr:colOff>1218251</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>96372</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>33618</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:colOff>26292</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>137057</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3694,12 +3719,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="55" idx="3"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1524000" y="5513294"/>
-          <a:ext cx="605118" cy="22412"/>
+          <a:off x="1474693" y="6214353"/>
+          <a:ext cx="647099" cy="40685"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3727,13 +3754,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>874059</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1101193</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>100423</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3798,13 +3825,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>40341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>760534</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>73529</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3869,13 +3896,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1627094</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>103094</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>16463</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>136282</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3940,13 +3967,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1600200</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>121024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1827334</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>154211</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4009,16 +4036,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1149723</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>6724</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9739</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>39912</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>292473</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>515297</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>157144</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4033,8 +4060,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5140698" y="5502649"/>
-          <a:ext cx="222091" cy="214163"/>
+          <a:off x="548915" y="7531475"/>
+          <a:ext cx="222824" cy="216361"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5068,6 +5095,459 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>987669</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>129383</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2908CFF6-D9BA-4687-BA73-9904C55C52A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="351692" y="6945923"/>
+          <a:ext cx="892419" cy="590979"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>234462</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>73269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>541460</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580EBA49-1E00-4F13-AF16-EA8CA712B8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="85" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="234462" y="6374423"/>
+          <a:ext cx="563440" cy="754673"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>249117</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580EBA49-1E00-4F13-AF16-EA8CA712B8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="249117" y="4772025"/>
+          <a:ext cx="112833" cy="1564298"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>541460</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>129383</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542193</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>153866</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{580EBA49-1E00-4F13-AF16-EA8CA712B8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="85" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="797902" y="7536902"/>
+          <a:ext cx="733" cy="207656"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>117231</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>51289</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83613</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>77150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="66 Rectángulo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2BD95EB-2284-4C40-8FFF-3FD565A9E5B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="117231" y="4842364"/>
+          <a:ext cx="223557" cy="216361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>115766</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13189</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>338590</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>39050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="66 Rectángulo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2BD95EB-2284-4C40-8FFF-3FD565A9E5B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="372208" y="4651131"/>
+          <a:ext cx="222824" cy="216361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>531934</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>143607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>754758</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>176795</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="66 Rectángulo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2BD95EB-2284-4C40-8FFF-3FD565A9E5B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="788376" y="7551126"/>
+          <a:ext cx="222824" cy="216361"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5514,10 +5994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L42"/>
+  <dimension ref="A2:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5542,7 +6022,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
@@ -5550,7 +6030,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
@@ -5566,42 +6046,48 @@
         <v>21</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="E7" s="10"/>
       <c r="I7" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="I8" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="I9" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="E10" s="11"/>
       <c r="I10" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
@@ -5613,361 +6099,384 @@
     <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="E13" s="10"/>
       <c r="H13" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H14" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>30</v>
-      </c>
       <c r="J17" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="F18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="H18" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="F19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="H19" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="8"/>
       <c r="H20" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="5" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J23" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="E27" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E28" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="C29" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C30" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C31" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C32" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C33" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C34" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C35" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C36" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C37" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C38" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C39" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C40" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="H26" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="C27" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C28" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C29" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C30" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C31" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C32" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="L32" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C33" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C34" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C35" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C36" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C37" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C38" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="E40" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C41" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="J41" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J42" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
presupuestos y r operativos
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15690" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="17550" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="158">
   <si>
     <t>pedidos</t>
   </si>
@@ -458,6 +459,57 @@
   </si>
   <si>
     <t>gas_detalle</t>
+  </si>
+  <si>
+    <t>costo_gasto</t>
+  </si>
+  <si>
+    <t>r_operativos</t>
+  </si>
+  <si>
+    <t>id_ro</t>
+  </si>
+  <si>
+    <t>ro_detalles</t>
+  </si>
+  <si>
+    <t>id_ro_de</t>
+  </si>
+  <si>
+    <t>id_ro1</t>
+  </si>
+  <si>
+    <t>inventario</t>
+  </si>
+  <si>
+    <t>ventas</t>
+  </si>
+  <si>
+    <t>g_operacion</t>
+  </si>
+  <si>
+    <t>margen</t>
+  </si>
+  <si>
+    <t>u_bruta</t>
+  </si>
+  <si>
+    <t>u_neta</t>
+  </si>
+  <si>
+    <t>dividendo</t>
+  </si>
+  <si>
+    <t>cxpagar</t>
+  </si>
+  <si>
+    <t>credito</t>
+  </si>
+  <si>
+    <t>efectivo</t>
+  </si>
+  <si>
+    <t>tarjeta</t>
   </si>
 </sst>
 </file>
@@ -508,7 +560,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,6 +645,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -606,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -662,6 +726,13 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5989,6 +6060,88 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+            </a:rPr>
+            <a:t>1:N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1262213</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133545</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="98" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9424147" y="9726706"/>
+          <a:ext cx="892419" cy="592986"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>1:N</a:t>
           </a:r>
@@ -6441,10 +6594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L62"/>
+  <dimension ref="A2:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6461,10 +6614,12 @@
     <col min="10" max="10" width="27.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="21" style="3" customWidth="1"/>
     <col min="12" max="12" width="24.7109375" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="3"/>
+    <col min="13" max="13" width="11.42578125" style="3"/>
+    <col min="14" max="14" width="21.140625" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
@@ -6472,7 +6627,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
@@ -6480,7 +6635,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
@@ -6488,23 +6643,29 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="N5" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="N6" s="28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>116</v>
       </c>
@@ -6514,8 +6675,11 @@
       <c r="I7" s="18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="N7" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C8" s="5" t="s">
         <v>117</v>
       </c>
@@ -6526,7 +6690,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
@@ -6537,31 +6701,40 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E10" s="10"/>
       <c r="I10" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="N12" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="E13" s="11"/>
       <c r="H13" s="18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="N13" s="28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E14" s="10"/>
       <c r="H14" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="N14" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
@@ -6569,8 +6742,11 @@
       <c r="H15" s="20" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="N15" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -6584,8 +6760,11 @@
       <c r="H16" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="N16" s="28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>114</v>
       </c>
@@ -6601,8 +6780,11 @@
       <c r="J17" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N17" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
@@ -6618,8 +6800,11 @@
       <c r="J18" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N18" s="28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>34</v>
       </c>
@@ -6635,8 +6820,11 @@
       <c r="J19" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N19" s="28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
@@ -6650,8 +6838,11 @@
       <c r="J20" s="17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N20" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>84</v>
       </c>
@@ -6664,8 +6855,11 @@
       <c r="J21" s="17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N21" s="28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="5" t="s">
         <v>41</v>
@@ -6679,8 +6873,11 @@
       <c r="J22" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N22" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>75</v>
       </c>
@@ -6690,16 +6887,22 @@
       <c r="J23" s="13" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N23" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="N24" s="28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>43</v>
       </c>
@@ -6709,8 +6912,11 @@
       <c r="L25" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="N25" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
@@ -6723,8 +6929,11 @@
       <c r="L26" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N26" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H27" s="7" t="s">
         <v>55</v>
       </c>
@@ -6735,7 +6944,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H28" s="7" t="s">
         <v>54</v>
       </c>
@@ -6746,7 +6955,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C29" s="12" t="s">
         <v>68</v>
       </c>
@@ -6757,7 +6966,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
         <v>31</v>
       </c>
@@ -6771,7 +6980,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C31" s="15" t="s">
         <v>69</v>
       </c>
@@ -6785,7 +6994,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C32" s="15" t="s">
         <v>72</v>
       </c>
@@ -7045,6 +7254,16 @@
       </c>
       <c r="E62" s="7" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C63" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C64" s="25" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pequeñas mejoras en presupuestos
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17550" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="18480" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="162">
   <si>
     <t>pedidos</t>
   </si>
@@ -510,6 +509,18 @@
   </si>
   <si>
     <t>tarjeta</t>
+  </si>
+  <si>
+    <t>id_pers4</t>
+  </si>
+  <si>
+    <t>id_pre_detalle_cat</t>
+  </si>
+  <si>
+    <t>cate_pre</t>
+  </si>
+  <si>
+    <t>pre_detalle_cat</t>
   </si>
 </sst>
 </file>
@@ -560,7 +571,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -657,6 +668,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -670,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -733,6 +750,7 @@
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5990,15 +6008,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>413644</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>157369</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1306063</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>27819</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6148,6 +6166,202 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1519948</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>38538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="99" name="10 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E1D4531-B4E5-4549-A8EC-0FC88AC5C515}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11586882" y="10399059"/>
+          <a:ext cx="892419" cy="598832"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1:N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1042147</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1703294</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="102" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12001500" y="8236324"/>
+          <a:ext cx="661147" cy="2173941"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1519948</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>97710</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="99" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12479301" y="10698475"/>
+          <a:ext cx="362641" cy="81584"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6594,10 +6808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N64"/>
+  <dimension ref="A2:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="H48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7179,91 +7393,117 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="G48" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C51" s="24" t="s">
+      <c r="I48" s="24" t="s">
         <v>138</v>
       </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="I49" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="I50" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11" ht="15" x14ac:dyDescent="0.25">
       <c r="E51" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C52" s="25" t="s">
-        <v>129</v>
-      </c>
+      <c r="I51" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E52" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C53" s="25" t="s">
-        <v>130</v>
-      </c>
+    <row r="53" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E53" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C54" s="25" t="s">
-        <v>137</v>
-      </c>
+    <row r="54" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E54" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="3:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C58" s="24" t="s">
+    <row r="55" spans="5:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="I55" s="24" t="s">
         <v>132</v>
       </c>
+      <c r="K55" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="I56" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="K56" s="25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="I57" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="K57" s="25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="5:11" ht="15" x14ac:dyDescent="0.25">
       <c r="E58" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C59" s="25" t="s">
-        <v>133</v>
-      </c>
+      <c r="I58" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="K58" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E59" s="7" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C60" s="26" t="s">
-        <v>134</v>
-      </c>
+      <c r="I59" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E60" s="17" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C61" s="25" t="s">
-        <v>6</v>
-      </c>
+      <c r="I60" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E61" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C62" s="25" t="s">
-        <v>95</v>
-      </c>
+      <c r="I61" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E62" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C63" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C64" s="25" t="s">
-        <v>22</v>
+      <c r="I62" s="25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="I63" s="26" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mas proveedor y pedidos
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19410" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="20340" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -6819,8 +6819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7307,7 +7307,7 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="30" t="s">
         <v>74</v>
       </c>
       <c r="E38" s="14" t="s">
@@ -7321,7 +7321,7 @@
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="30" t="s">
         <v>76</v>
       </c>
       <c r="E39" s="14" t="s">
@@ -7335,10 +7335,10 @@
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="30" t="s">
         <v>64</v>
       </c>
       <c r="H40" s="7" t="s">
@@ -7352,7 +7352,7 @@
       <c r="C41" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="30" t="s">
         <v>77</v>
       </c>
       <c r="H41" s="7" t="s">
@@ -7363,7 +7363,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="30" t="s">
         <v>80</v>
       </c>
       <c r="H42" s="7" t="s">

</xml_diff>

<commit_message>
Nuevo modulo ventas diarias
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28710" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="29640" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="194">
   <si>
     <t>pedidos</t>
   </si>
@@ -490,12 +490,6 @@
     <t>margen</t>
   </si>
   <si>
-    <t>u_bruta</t>
-  </si>
-  <si>
-    <t>u_neta</t>
-  </si>
-  <si>
     <t>dividendo</t>
   </si>
   <si>
@@ -619,16 +613,10 @@
     <t>id_pers5</t>
   </si>
   <si>
-    <t>ro_detalles_inversion</t>
-  </si>
-  <si>
-    <t>id_ro_de_inv</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>id_ro_de1</t>
+    <t>comentario_inversion</t>
+  </si>
+  <si>
+    <t>inversion</t>
   </si>
 </sst>
 </file>
@@ -7475,88 +7463,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1016244</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>36054</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="119" name="15 Rombo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="21745575" y="2771775"/>
-          <a:ext cx="892419" cy="607554"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>1:1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8003,10 +7909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P63"/>
+  <dimension ref="A2:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="J10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8026,11 +7932,10 @@
     <col min="13" max="13" width="11.42578125" style="3"/>
     <col min="14" max="14" width="21.140625" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="3"/>
+    <col min="16" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
@@ -8038,10 +7943,10 @@
         <v>110</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
@@ -8049,10 +7954,10 @@
         <v>109</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
@@ -8060,38 +7965,38 @@
         <v>46</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N5" s="27" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>95</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
@@ -8099,7 +8004,7 @@
         <v>40</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>103</v>
@@ -8108,7 +8013,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C8" s="5" t="s">
         <v>115</v>
       </c>
@@ -8120,7 +8025,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>116</v>
       </c>
@@ -8135,7 +8040,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
         <v>117</v>
       </c>
@@ -8144,10 +8049,10 @@
         <v>22</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
@@ -8156,28 +8061,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="E12" s="10"/>
       <c r="K12" s="17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N12" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="E13" s="11"/>
       <c r="H13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N13" s="28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E14" s="10"/>
       <c r="H14" s="19" t="s">
         <v>24</v>
@@ -8186,7 +8091,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
@@ -8197,11 +8102,8 @@
       <c r="N15" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="P15" s="27" t="s">
-        <v>194</v>
-      </c>
     </row>
-    <row r="16" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -8218,11 +8120,8 @@
       <c r="N16" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="P16" s="28" t="s">
-        <v>195</v>
-      </c>
     </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>114</v>
       </c>
@@ -8241,11 +8140,8 @@
       <c r="N17" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="P17" s="29" t="s">
-        <v>197</v>
-      </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
@@ -8264,11 +8160,8 @@
       <c r="N18" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="P18" s="28" t="s">
-        <v>196</v>
-      </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>34</v>
       </c>
@@ -8288,7 +8181,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
@@ -8296,7 +8189,7 @@
         <v>42</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>22</v>
@@ -8308,7 +8201,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>84</v>
       </c>
@@ -8325,7 +8218,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="5" t="s">
         <v>41</v>
@@ -8343,7 +8236,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>75</v>
       </c>
@@ -8357,9 +8250,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B24" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>90</v>
@@ -8368,7 +8261,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>83</v>
       </c>
@@ -8379,10 +8272,10 @@
         <v>96</v>
       </c>
       <c r="N25" s="28" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>43</v>
       </c>
@@ -8396,10 +8289,10 @@
         <v>97</v>
       </c>
       <c r="N26" s="28" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>22</v>
       </c>
@@ -8413,7 +8306,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H28" s="7" t="s">
         <v>54</v>
       </c>
@@ -8424,7 +8317,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C29" s="12" t="s">
         <v>68</v>
       </c>
@@ -8435,7 +8328,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C30" s="14" t="s">
         <v>31</v>
       </c>
@@ -8449,7 +8342,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C31" s="15" t="s">
         <v>69</v>
       </c>
@@ -8462,11 +8355,8 @@
       <c r="L31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="N31" s="27" t="s">
-        <v>164</v>
-      </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C32" s="15" t="s">
         <v>72</v>
       </c>
@@ -8479,8 +8369,8 @@
       <c r="L32" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N32" s="28" t="s">
-        <v>167</v>
+      <c r="N32" s="27" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -8508,7 +8398,7 @@
         <v>57</v>
       </c>
       <c r="N34" s="28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
@@ -8522,7 +8412,7 @@
         <v>50</v>
       </c>
       <c r="N35" s="28" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -8539,7 +8429,9 @@
       <c r="J36" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="N36" s="10"/>
+      <c r="N36" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C37" s="14" t="s">
@@ -8554,8 +8446,9 @@
       <c r="J37" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="N37" s="10"/>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C38" s="30" t="s">
         <v>74</v>
       </c>
@@ -8568,11 +8461,8 @@
       <c r="J38" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="N38" s="27" t="s">
-        <v>168</v>
-      </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="C39" s="30" t="s">
         <v>76</v>
       </c>
@@ -8585,8 +8475,8 @@
       <c r="J39" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="N39" s="28" t="s">
-        <v>169</v>
+      <c r="N39" s="27" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -8603,7 +8493,7 @@
         <v>95</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -8620,7 +8510,7 @@
         <v>40</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -8634,7 +8524,7 @@
         <v>22</v>
       </c>
       <c r="N42" s="28" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -8644,6 +8534,9 @@
       <c r="H43" s="7" t="s">
         <v>121</v>
       </c>
+      <c r="N43" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H44" s="7" t="s">
@@ -8688,7 +8581,7 @@
         <v>138</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
@@ -8696,7 +8589,7 @@
         <v>129</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
@@ -8704,7 +8597,7 @@
         <v>130</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="3:11" ht="15" x14ac:dyDescent="0.25">
@@ -8712,13 +8605,13 @@
         <v>139</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I51" s="25" t="s">
         <v>137</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.2">
@@ -8726,10 +8619,10 @@
         <v>131</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.2">
@@ -8737,10 +8630,10 @@
         <v>130</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.2">
@@ -8748,10 +8641,10 @@
         <v>137</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="55" spans="3:11" ht="15" x14ac:dyDescent="0.25">
@@ -8759,13 +8652,13 @@
         <v>40</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I55" s="24" t="s">
         <v>132</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.2">
@@ -8773,18 +8666,18 @@
         <v>22</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I56" s="25" t="s">
         <v>133</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.2">
       <c r="G57" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I57" s="26" t="s">
         <v>134</v>
@@ -8838,7 +8731,7 @@
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.2">
       <c r="I63" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalizacion de ventas diarias
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="30570" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="197">
   <si>
     <t>pedidos</t>
   </si>
@@ -617,6 +617,15 @@
   </si>
   <si>
     <t>inversion</t>
+  </si>
+  <si>
+    <t>ventas_diarias</t>
+  </si>
+  <si>
+    <t>id_ven_dia</t>
+  </si>
+  <si>
+    <t>id_fecha1</t>
   </si>
 </sst>
 </file>
@@ -783,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -850,6 +859,9 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7436,6 +7448,206 @@
         <a:xfrm flipH="1">
           <a:off x="7940919" y="6768353"/>
           <a:ext cx="3029640" cy="1736449"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>621927</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>32497</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1514346</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>87601</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15178368" y="10117791"/>
+          <a:ext cx="892419" cy="604192"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:N</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1068137</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>32497</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="120" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="119" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14556441" y="8987118"/>
+          <a:ext cx="1068137" cy="1130673"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1068137</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>87601</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="121" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="119" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15624578" y="10721983"/>
+          <a:ext cx="780834" cy="618370"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7911,8 +8123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="H40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7932,7 +8144,8 @@
     <col min="13" max="13" width="11.42578125" style="3"/>
     <col min="14" max="14" width="21.140625" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="3"/>
+    <col min="16" max="16" width="17.7109375" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15" x14ac:dyDescent="0.25">
@@ -8705,12 +8918,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:11" ht="15" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
         <v>136</v>
       </c>
       <c r="I60" s="30" t="s">
         <v>141</v>
+      </c>
+      <c r="K60" s="32" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.2">
@@ -8720,6 +8936,9 @@
       <c r="I61" s="25" t="s">
         <v>22</v>
       </c>
+      <c r="K61" s="14" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C62" s="7" t="s">
@@ -8728,10 +8947,16 @@
       <c r="I62" s="25" t="s">
         <v>38</v>
       </c>
+      <c r="K62" s="15" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.2">
       <c r="I63" s="26" t="s">
         <v>156</v>
+      </c>
+      <c r="K63" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inicio caja de persona
</commit_message>
<xml_diff>
--- a/bd/bd.xlsx
+++ b/bd/bd.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30570" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="33360" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="209">
   <si>
     <t>pedidos</t>
   </si>
@@ -626,6 +626,42 @@
   </si>
   <si>
     <t>id_fecha1</t>
+  </si>
+  <si>
+    <t>moneda</t>
+  </si>
+  <si>
+    <t>id_efectivo_en_caja</t>
+  </si>
+  <si>
+    <t>efectivo_en_caja</t>
+  </si>
+  <si>
+    <t>venta_diaria</t>
+  </si>
+  <si>
+    <t>id_venta_diaria</t>
+  </si>
+  <si>
+    <t>id_cuadre_caja_completo</t>
+  </si>
+  <si>
+    <t>id_pers6</t>
+  </si>
+  <si>
+    <t>id_cuadre_caja_completo1</t>
+  </si>
+  <si>
+    <t>id_cuadre_caja_completo2</t>
+  </si>
+  <si>
+    <t>id_cuadre_caja_completo3</t>
+  </si>
+  <si>
+    <t>id_cuadre_caja_completo4</t>
+  </si>
+  <si>
+    <t>cuadre_de_caja_completo</t>
   </si>
 </sst>
 </file>
@@ -792,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -862,6 +898,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7675,6 +7712,591 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1183772</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>155958</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="122" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18097500" y="8180294"/>
+          <a:ext cx="892419" cy="604193"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="123" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12853147" y="5815853"/>
+          <a:ext cx="1703294" cy="1972235"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>291353</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>33156</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="124" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="122" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14578853" y="7788088"/>
+          <a:ext cx="3518647" cy="694303"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1183772</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>33156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1848970</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="33 Conector recto">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2E09284-0C72-4EFA-980E-18D08D2CA024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="122" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18989919" y="8482391"/>
+          <a:ext cx="3074463" cy="1535668"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1430301</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>66311</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="126" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20753294" y="8281147"/>
+          <a:ext cx="892419" cy="604193"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>17928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1425818</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>73033</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24480370" y="7918075"/>
+          <a:ext cx="892419" cy="604193"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1851211</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>69475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>883454</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>124580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22066623" y="5963769"/>
+          <a:ext cx="892419" cy="604193"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>961463</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>42582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1853882</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>108892</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="130" name="15 Rombo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023B7A06-6FB0-46AE-A2A1-37B74AD98C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23037051" y="6676464"/>
+          <a:ext cx="892419" cy="604193"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8121,10 +8743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N63"/>
+  <dimension ref="A2:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView tabSelected="1" topLeftCell="I29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8142,9 +8764,9 @@
     <col min="11" max="11" width="21" style="3" customWidth="1"/>
     <col min="12" max="12" width="24.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" style="3"/>
-    <col min="14" max="14" width="21.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="28" style="3" customWidth="1"/>
+    <col min="16" max="16" width="28.85546875" style="3" customWidth="1"/>
     <col min="17" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -8586,7 +9208,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C33" s="16" t="s">
         <v>63</v>
       </c>
@@ -8600,7 +9222,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="C34" s="14" t="s">
         <v>71</v>
       </c>
@@ -8610,11 +9232,14 @@
       <c r="H34" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N34" s="28" t="s">
-        <v>163</v>
+      <c r="N34" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="P34" s="27" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C35" s="14" t="s">
         <v>73</v>
       </c>
@@ -8625,10 +9250,13 @@
         <v>50</v>
       </c>
       <c r="N35" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+      <c r="P35" s="28" t="s">
+        <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="C36" s="14" t="s">
         <v>78</v>
@@ -8643,10 +9271,13 @@
         <v>94</v>
       </c>
       <c r="N36" s="28" t="s">
-        <v>22</v>
+        <v>164</v>
+      </c>
+      <c r="P36" s="33" t="s">
+        <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C37" s="14" t="s">
         <v>70</v>
       </c>
@@ -8659,9 +9290,14 @@
       <c r="J37" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="N37" s="10"/>
+      <c r="N37" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37" s="28" t="s">
+        <v>197</v>
+      </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C38" s="30" t="s">
         <v>74</v>
       </c>
@@ -8674,8 +9310,12 @@
       <c r="J38" s="17" t="s">
         <v>93</v>
       </c>
+      <c r="N38" s="10"/>
+      <c r="P38" s="28" t="s">
+        <v>199</v>
+      </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C39" s="30" t="s">
         <v>76</v>
       </c>
@@ -8688,11 +9328,8 @@
       <c r="J39" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="N39" s="27" t="s">
-        <v>166</v>
-      </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="C40" s="30" t="s">
         <v>79</v>
       </c>
@@ -8705,11 +9342,14 @@
       <c r="J40" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="N40" s="28" t="s">
-        <v>167</v>
+      <c r="N40" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="P40" s="27" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C41" s="14" t="s">
         <v>22</v>
       </c>
@@ -8723,10 +9363,13 @@
         <v>40</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="P41" s="28" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E42" s="30" t="s">
         <v>80</v>
       </c>
@@ -8736,11 +9379,14 @@
       <c r="J42" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N42" s="28" t="s">
-        <v>164</v>
+      <c r="N42" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="P42" s="33" t="s">
+        <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E43" s="14" t="s">
         <v>22</v>
       </c>
@@ -8748,15 +9394,21 @@
         <v>121</v>
       </c>
       <c r="N43" s="28" t="s">
-        <v>22</v>
+        <v>168</v>
+      </c>
+      <c r="P43" s="28" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H44" s="7" t="s">
         <v>122</v>
       </c>
+      <c r="N44" s="28" t="s">
+        <v>164</v>
+      </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
         <v>111</v>
       </c>
@@ -8766,8 +9418,11 @@
       <c r="H45" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="N45" s="28" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B46" s="23" t="s">
         <v>112</v>
       </c>
@@ -8775,7 +9430,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B47" s="23" t="s">
         <v>113</v>
       </c>
@@ -8783,7 +9438,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="23" t="s">
         <v>22</v>
       </c>
@@ -8797,7 +9452,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I49" s="25" t="s">
         <v>129</v>
       </c>
@@ -8805,7 +9460,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I50" s="25" t="s">
         <v>130</v>
       </c>
@@ -8813,7 +9468,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" ht="15" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
         <v>139</v>
       </c>
@@ -8827,7 +9482,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C52" s="7" t="s">
         <v>131</v>
       </c>
@@ -8838,7 +9493,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:15" ht="15" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="s">
         <v>130</v>
       </c>
@@ -8848,8 +9503,11 @@
       <c r="K53" s="7" t="s">
         <v>183</v>
       </c>
+      <c r="O53" s="27" t="s">
+        <v>208</v>
+      </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C54" s="7" t="s">
         <v>137</v>
       </c>
@@ -8859,8 +9517,11 @@
       <c r="K54" s="7" t="s">
         <v>184</v>
       </c>
+      <c r="O54" s="28" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="55" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:15" ht="15" x14ac:dyDescent="0.25">
       <c r="E55" s="7" t="s">
         <v>40</v>
       </c>
@@ -8873,8 +9534,11 @@
       <c r="K55" s="7" t="s">
         <v>185</v>
       </c>
+      <c r="O55" s="29" t="s">
+        <v>203</v>
+      </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:15" x14ac:dyDescent="0.2">
       <c r="E56" s="7" t="s">
         <v>22</v>
       </c>
@@ -8888,7 +9552,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.2">
       <c r="G57" s="25" t="s">
         <v>158</v>
       </c>
@@ -8899,7 +9563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:15" ht="15" x14ac:dyDescent="0.25">
       <c r="C58" s="6" t="s">
         <v>140</v>
       </c>
@@ -8910,7 +9574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C59" s="7" t="s">
         <v>135</v>
       </c>
@@ -8918,7 +9582,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60" spans="3:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:15" ht="15" x14ac:dyDescent="0.25">
       <c r="C60" s="17" t="s">
         <v>136</v>
       </c>
@@ -8929,7 +9593,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C61" s="7" t="s">
         <v>6</v>
       </c>
@@ -8940,7 +9604,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C62" s="7" t="s">
         <v>95</v>
       </c>
@@ -8951,7 +9615,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:15" x14ac:dyDescent="0.2">
       <c r="I63" s="26" t="s">
         <v>156</v>
       </c>

</xml_diff>